<commit_message>
vault backup: 2025-06-30 11:09:39
</commit_message>
<xml_diff>
--- a/Маркированные и подакцизные товары.xlsx
+++ b/Маркированные и подакцизные товары.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\OBSVLT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OBSVLT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D156C343-E363-4AEC-B2E6-57491ACC876C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE16A0D-9D26-4293-8BF2-D56923474B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -716,23 +716,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1048,10 +1045,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="142.5" thickBot="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1098,10 +1095,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1110,10 +1107,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1122,10 +1119,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1160,10 +1157,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1172,10 +1169,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1260,10 +1257,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1334,10 +1331,10 @@
       <c r="D23" s="20"/>
     </row>
     <row r="24" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="22"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1371,17 +1368,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="D22:D23"/>
@@ -1389,6 +1375,17 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1397,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F08E9C-1A2C-4B88-A0A5-82884D7265B8}">
-  <dimension ref="A1:C392"/>
+  <dimension ref="A1:E392"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1422,7 +1419,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1433,7 +1430,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="29"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="10" t="s">
         <v>54</v>
       </c>
@@ -1442,7 +1439,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30">
-      <c r="A4" s="29"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="10" t="s">
         <v>57</v>
       </c>
@@ -1451,135 +1448,135 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="29"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="10" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="29"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A8" s="30"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A10" s="29"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="31"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="29"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="32"/>
+      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="32"/>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="32"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A15" s="30"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="32"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>69</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A17" s="30"/>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A17" s="29"/>
       <c r="B17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="33"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="28" t="s">
+      <c r="C17" s="32"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="27" t="s">
         <v>78</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="29"/>
+    <row r="19" spans="1:5">
+      <c r="A19" s="28"/>
       <c r="B19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="32"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A20" s="30"/>
+      <c r="C19" s="31"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A20" s="29"/>
       <c r="B20" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="33"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="28" t="s">
+      <c r="C20" s="32"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="27" t="s">
         <v>77</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -1589,29 +1586,29 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="29"/>
+    <row r="22" spans="1:5">
+      <c r="A22" s="28"/>
       <c r="B22" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="11"/>
     </row>
-    <row r="23" spans="1:3" ht="30">
-      <c r="A23" s="29"/>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="28"/>
       <c r="B23" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C23" s="11"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A24" s="30"/>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A24" s="29"/>
       <c r="B24" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C24" s="13"/>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="27" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -1621,15 +1618,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A26" s="30"/>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A26" s="29"/>
       <c r="B26" s="12" t="s">
         <v>80</v>
       </c>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A27" s="27" t="s">
         <v>90</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -1639,8 +1636,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="29"/>
+    <row r="28" spans="1:5">
+      <c r="A28" s="28"/>
       <c r="B28" s="10" t="s">
         <v>83</v>
       </c>
@@ -1648,8 +1645,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32.25" customHeight="1">
-      <c r="A29" s="29"/>
+    <row r="29" spans="1:5" ht="32.25" customHeight="1">
+      <c r="A29" s="28"/>
       <c r="B29" s="10" t="s">
         <v>84</v>
       </c>
@@ -1657,8 +1654,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30">
-      <c r="A30" s="29"/>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="28"/>
       <c r="B30" s="10" t="s">
         <v>85</v>
       </c>
@@ -1666,8 +1663,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="45.75" thickBot="1">
-      <c r="A31" s="30"/>
+    <row r="31" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A31" s="29"/>
       <c r="B31" s="12" t="s">
         <v>86</v>
       </c>
@@ -1675,8 +1672,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="27" t="s">
         <v>95</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -1685,9 +1682,10 @@
       <c r="C32" s="9" t="s">
         <v>93</v>
       </c>
+      <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="29"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="15" t="s">
         <v>80</v>
       </c>
@@ -1696,7 +1694,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A34" s="30"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="16"/>
       <c r="C34" s="13" t="s">
         <v>81</v>
@@ -1706,8 +1704,8 @@
       <c r="A35" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
     </row>
     <row r="36" spans="1:3" s="18" customFormat="1">
       <c r="A36" s="17"/>

</xml_diff>

<commit_message>
vault backup: 2025-06-30 13:48:49
</commit_message>
<xml_diff>
--- a/Маркированные и подакцизные товары.xlsx
+++ b/Маркированные и подакцизные товары.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OBSVLT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE16A0D-9D26-4293-8BF2-D56923474B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1176F49-FF34-485A-8BA5-6C280B7BC86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="103">
   <si>
     <t>Товар</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>Обувь</t>
+  </si>
+  <si>
+    <t>Молочная продукция</t>
   </si>
 </sst>
 </file>
@@ -716,20 +719,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1045,10 +1048,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="142.5" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1095,10 +1098,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1107,10 +1110,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1119,10 +1122,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1157,10 +1160,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1169,10 +1172,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1257,10 +1260,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1331,10 +1334,10 @@
       <c r="D23" s="20"/>
     </row>
     <row r="24" spans="1:4" ht="43.5" thickBot="1">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="25"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1368,6 +1371,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="D22:D23"/>
@@ -1375,17 +1389,6 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1394,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F08E9C-1A2C-4B88-A0A5-82884D7265B8}">
-  <dimension ref="A1:E392"/>
+  <dimension ref="A1:E393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:C35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1468,306 +1471,308 @@
       </c>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="28"/>
+      <c r="B8" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A9" s="29"/>
+      <c r="B9" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="13"/>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A9" s="27" t="s">
+      <c r="C9" s="13"/>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A10" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C10" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A11" s="28"/>
+      <c r="B11" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="31"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="27" t="s">
+      <c r="C11" s="31"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C12" s="30" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="28"/>
       <c r="B13" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="31"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="28"/>
       <c r="B14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="31"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="12" t="s">
+      <c r="C15" s="31"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A16" s="29"/>
+      <c r="B16" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="32"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="27" t="s">
+      <c r="C16" s="32"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C17" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="12" t="s">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A18" s="29"/>
+      <c r="B18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="32"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="27" t="s">
+      <c r="C18" s="32"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C19" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="28"/>
-      <c r="B19" s="10" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="28"/>
+      <c r="B20" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="31"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A20" s="29"/>
-      <c r="B20" s="12" t="s">
+      <c r="C20" s="31"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A21" s="29"/>
+      <c r="B21" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="32"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="27" t="s">
+      <c r="C21" s="32"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B22" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="28"/>
-      <c r="B22" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:3">
       <c r="A23" s="28"/>
       <c r="B23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" ht="30">
+      <c r="A24" s="28"/>
+      <c r="B24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A24" s="29"/>
-      <c r="B24" s="12" t="s">
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A25" s="29"/>
+      <c r="B25" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="13"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="27" t="s">
+      <c r="C25" s="13"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="12" t="s">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A27" s="29"/>
+      <c r="B27" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="13"/>
-    </row>
-    <row r="27" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A27" s="27" t="s">
+      <c r="C27" s="13"/>
+    </row>
+    <row r="28" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A28" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="28"/>
-      <c r="B28" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="32.25" customHeight="1">
+    <row r="29" spans="1:3">
       <c r="A29" s="28"/>
       <c r="B29" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="32.25" customHeight="1">
       <c r="A30" s="28"/>
       <c r="B30" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30">
+      <c r="A31" s="28"/>
+      <c r="B31" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="12" t="s">
+    <row r="32" spans="1:3" ht="45.75" thickBot="1">
+      <c r="A32" s="29"/>
+      <c r="B32" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C32" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="27" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B33" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E32" s="18"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="15" t="s">
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="28"/>
+      <c r="B34" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="13" t="s">
+    <row r="35" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A35" s="29"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="60" customHeight="1">
-      <c r="A35" s="26" t="s">
+    <row r="36" spans="1:5" ht="60" customHeight="1">
+      <c r="A36" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-    </row>
-    <row r="36" spans="1:3" s="18" customFormat="1">
-      <c r="A36" s="17"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" s="18" customFormat="1">
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+    </row>
+    <row r="37" spans="1:5" s="18" customFormat="1">
       <c r="A37" s="17"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" s="18" customFormat="1">
+    <row r="38" spans="1:5" s="18" customFormat="1">
       <c r="A38" s="17"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" s="18" customFormat="1">
+    <row r="39" spans="1:5" s="18" customFormat="1">
       <c r="A39" s="17"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" s="18" customFormat="1">
+    <row r="40" spans="1:5" s="18" customFormat="1">
       <c r="A40" s="17"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" s="18" customFormat="1">
+    <row r="41" spans="1:5" s="18" customFormat="1">
       <c r="A41" s="17"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" s="18" customFormat="1">
+    <row r="42" spans="1:5" s="18" customFormat="1">
       <c r="A42" s="17"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" s="18" customFormat="1">
+    <row r="43" spans="1:5" s="18" customFormat="1">
       <c r="A43" s="17"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" s="18" customFormat="1">
+    <row r="44" spans="1:5" s="18" customFormat="1">
       <c r="A44" s="17"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" s="18" customFormat="1">
+    <row r="45" spans="1:5" s="18" customFormat="1">
       <c r="A45" s="17"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" s="18" customFormat="1">
+    <row r="46" spans="1:5" s="18" customFormat="1">
       <c r="A46" s="17"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" s="18" customFormat="1">
+    <row r="47" spans="1:5" s="18" customFormat="1">
       <c r="A47" s="17"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" s="18" customFormat="1">
+    <row r="48" spans="1:5" s="18" customFormat="1">
       <c r="A48" s="17"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -3492,22 +3497,27 @@
       <c r="B392" s="4"/>
       <c r="C392" s="4"/>
     </row>
+    <row r="393" spans="1:3" s="18" customFormat="1">
+      <c r="A393" s="17"/>
+      <c r="B393" s="4"/>
+      <c r="C393" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>